<commit_message>
Review the UX comments
</commit_message>
<xml_diff>
--- a/Documents/TestCasesAndBugReport.xlsx
+++ b/Documents/TestCasesAndBugReport.xlsx
@@ -5,20 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InstaBugTask\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BosyShafey\Desktop\BosyShafey-master\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E68FD2D-3432-43ED-B8F0-95CE7CB51275}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC65A379-5C3C-471A-A3DB-9DE13B5D14D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7B5E37A7-6117-4840-83DD-C655CC8B3E4E}"/>
   </bookViews>
   <sheets>
-    <sheet name="First part_TC" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Report " sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
   <si>
     <t xml:space="preserve">Monfey_TC_ID </t>
   </si>
@@ -58,15 +57,6 @@
 Android Version: 9 </t>
   </si>
   <si>
-    <t xml:space="preserve">1- install the app using this Link
- https://play.google.com/store/apps/details?id=com.monefy.app.lite
-2-open the monfey application 
-click on the button + on the right hand side 
-3-Enter the the date 
-4-
-</t>
-  </si>
-  <si>
     <t>Adding new income</t>
   </si>
   <si>
@@ -76,12 +66,6 @@
     <t xml:space="preserve">verify that the user can add New Income category  </t>
   </si>
   <si>
-    <t xml:space="preserve">changing the date from the income tab </t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify that the user can click on the date , and change the </t>
-  </si>
-  <si>
     <t>Monfey_TC_02</t>
   </si>
   <si>
@@ -130,9 +114,6 @@
     <t xml:space="preserve">Severity </t>
   </si>
   <si>
-    <t xml:space="preserve">change the main currency </t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that the user can add new expense </t>
   </si>
   <si>
@@ -142,9 +123,6 @@
     <t xml:space="preserve">Add new income category </t>
   </si>
   <si>
-    <t xml:space="preserve">choosing the expense category </t>
-  </si>
-  <si>
     <t xml:space="preserve">verify that the user can choose the category of expense </t>
   </si>
   <si>
@@ -157,18 +135,12 @@
     <t xml:space="preserve">Validate that the user can change the currency </t>
   </si>
   <si>
-    <t xml:space="preserve">reflecting of changing the currency </t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that changing the currency reflecting on the balance currency </t>
   </si>
   <si>
     <t xml:space="preserve">Verify that the user can add the amount of cash payment </t>
   </si>
   <si>
-    <t xml:space="preserve">clicking on Balance on the  Home page of the application </t>
-  </si>
-  <si>
     <t xml:space="preserve">clicking on the Balance button shall list all expenses </t>
   </si>
   <si>
@@ -191,9 +163,6 @@
   </si>
   <si>
     <t>OppoF11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The line(connection) between the expense and the chart doesn't appear after entering the values for some expenses </t>
   </si>
   <si>
     <t>Salary: 1020$
@@ -222,33 +191,10 @@
     <t>Monfey_03</t>
   </si>
   <si>
-    <t xml:space="preserve">there is a UI issue on the right menu beside the balance, the UI menu button exchanged with another  button on the menu itself, 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the button shall shown the list of expenses , </t>
-  </si>
-  <si>
     <t xml:space="preserve">Low </t>
   </si>
   <si>
     <t>Medium</t>
-  </si>
-  <si>
-    <t>Video name: 
-Video_Monfey_03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expenses details </t>
-  </si>
-  <si>
-    <t>Validate that the user can view all expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ability to add several accounts per user using cash payment method </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ability to add several accounts per user using cash Mastercard method </t>
   </si>
   <si>
     <t xml:space="preserve">Verify that the user can add the amount of Mastercard payment </t>
@@ -262,12 +208,6 @@
 6-click on the right button beside the balance button </t>
   </si>
   <si>
-    <t xml:space="preserve">the button doesn't show the list of expenses. And shall appeared as a menu button </t>
-  </si>
-  <si>
-    <t>the user will impacted, he/she will click on useless button ,</t>
-  </si>
-  <si>
     <t>BugID</t>
   </si>
   <si>
@@ -278,9 +218,6 @@
   </si>
   <si>
     <t xml:space="preserve">Attachment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testcase </t>
   </si>
   <si>
     <t xml:space="preserve">Assigned to </t>
@@ -297,21 +234,6 @@
     <t xml:space="preserve">The line between the radial menu (chart) shall be from the chart to  all expenses , represented the percentage from  the user balance </t>
   </si>
   <si>
-    <t>there are some expenses with no line , those expenses are entertainment, transport, sports and car</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the user will not impacted critically with this issue , but it is a bad user experience to visualize with this issue </t>
-  </si>
-  <si>
-    <t>reference to those files 
-1-Bug_1.jpeg
-2-Bug_data_1.jpeg
-3-Bug_data_2.jpeg</t>
-  </si>
-  <si>
-    <t>There is missing option on iPhone for left side menu , The interval option appeared on Android but doesn't appear on iPhone</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-open monfey application 
 2-click on the left side menu 
 3-check the menu appeared 
@@ -319,18 +241,163 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">the appeared menu shall be the same for android and iPhone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">the appeared menu in iPhone missing the interval option </t>
-  </si>
-  <si>
     <t xml:space="preserve">The iPhone users will not be able to query the application by date range </t>
   </si>
   <si>
-    <t>reference to :
-Iphone-screen.jpeg
-Android_screen.jpeg</t>
+    <t>Monfey_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The application rotation doesn't work </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The application still as it is with no rotation </t>
+  </si>
+  <si>
+    <t>Testcase _ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The line(connection) between the expense and the chart doesn't appear after entering the values for expenses </t>
+  </si>
+  <si>
+    <t>There are some expenses with no line , those expenses are entertainment, transport, sports and car</t>
+  </si>
+  <si>
+    <t>Salary: 1020$
+savings:261</t>
+  </si>
+  <si>
+    <t>Reference to those files `
+1-Bug_screens-Videos/Bug_1.jepeg
+2-Bug_screens-Videos/Bug_data_1.jpeg
+3-Bug_screens-Videos/Bug_data_2.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user will not impacted critically with this issue , but it is a bad user experience to visualize with this issue </t>
+  </si>
+  <si>
+    <t>Reference to :
+Bug_screens-Videos/Iphone-screen.jpeg
+Bug_screens-Videos/Android_screen.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The appeared menu in iPhone missing the interval option </t>
+  </si>
+  <si>
+    <t>There is a missing option on iPhone for left side menu , The interval option appeared on Android but doesn't appear on iPhone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The appeared menu shall be the same for android and iPhone </t>
+  </si>
+  <si>
+    <t>Video name: 
+Bug_screens-Videos/Video_Monfey_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a UI issue on the right menu beside the balance, the UI menu button exchanged with another  button from the menu itself. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The button shall show the list of expenses , the button shall appear as a menu button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The button doesn't show the list of expenses. And doesn't  appear as a menu button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user will impacted, he/she will click on a button , with any new action </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Make the Auto rotate on 
+2-Open Monfey App 
+3-Rotaite the Mobile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The application shall be rotated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The application behavior has no rotation experience </t>
+  </si>
+  <si>
+    <t>verify that the user can click on the date , and change it as needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the user can view all expenses details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the main currency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reflecting of changing the currency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to add several accounts per user using cash Mastercard method </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to add several accounts per user using cash payment method </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expenses details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicking on Balance on the  Home page of the application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choosing the expense category </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changing the date from the income tab </t>
+  </si>
+  <si>
+    <t>Monfey_TC_14</t>
+  </si>
+  <si>
+    <t>Monfey_TC_15</t>
+  </si>
+  <si>
+    <t>Monfey_TC_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability of control the balance for  interval </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability of transfer a balance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can transfer balance from Mastercard to another one </t>
+  </si>
+  <si>
+    <t>Monfey_TC_17</t>
+  </si>
+  <si>
+    <t>Monfey_TC_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to restore the data from the data backup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can create a data backup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to save the data backup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can restore the data from the data backup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to clear the data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can clear his/her data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- install the app using this Link
+ https://play.google.com/store/apps/details?id=com.monefy.app.lite
+2-open the monfey application 
+click on the button + on the right hand side 
+3-Enter the  date 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user can add a balance for interval </t>
   </si>
 </sst>
 </file>
@@ -729,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84037EAD-22CA-4A7F-87AD-5CB822FEB73B}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -771,10 +838,10 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="144" x14ac:dyDescent="0.3">
@@ -782,145 +849,200 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -932,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964D0DCB-D2D9-407D-A649-C3E9B41D8F6E}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,156 +1070,185 @@
     <col min="6" max="6" width="17.44140625" customWidth="1"/>
     <col min="9" max="9" width="19.109375" customWidth="1"/>
     <col min="10" max="10" width="27" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="37.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.44140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="16.44140625" customWidth="1"/>
     <col min="14" max="14" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="N1" s="7" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>